<commit_message>
added Grey to xlsx
</commit_message>
<xml_diff>
--- a/gtaa_lab_v1.xlsx
+++ b/gtaa_lab_v1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamah/Programming/gtaa_N7K/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27504E95-B42A-F842-A948-0A62B23D9141}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="7700" windowWidth="35920" windowHeight="17720" xr2:uid="{0D690BAF-086B-8F44-B0C2-57543FF732B6}"/>
+    <workbookView xWindow="5400" yWindow="7695" windowWidth="35925" windowHeight="17715"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>de Guzman,Christian</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{A5E84E29-4B12-0940-A15B-D051FDDFF363}">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{12EA7377-233F-374D-B8A7-25CACA3FB892}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{E4889244-C6CD-4A4D-916C-23D2A52696BF}">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{D0E876DF-42B2-F34C-BF12-E6A266999F90}">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{B04FFA60-543A-9642-93D5-93767FAEC3B1}">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -275,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{06ACB2C9-1675-A848-BAB8-CAA1E62C7203}">
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -368,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{786BEFDD-5399-9440-B615-6DB0F070273B}">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>VRF-Name</t>
   </si>
@@ -562,10 +561,6 @@
   </si>
   <si>
     <t>IFT-Static-Routes</t>
-  </si>
-  <si>
-    <t>GREY
-(Yes/No)</t>
   </si>
   <si>
     <t>AIR-CHINA</t>
@@ -594,12 +589,15 @@
   <si>
     <t>10.155.108.0/24 Vlan2225 172.16.2.30
 10.201.7.0/24 Vlan2225 172.16.2.30</t>
+  </si>
+  <si>
+    <t>GREY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1005,19 +1003,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDCB523-1A96-5442-B28D-58271A369B0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="29.83203125" customWidth="1"/>
+    <col min="14" max="14" width="29.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,51 +1113,54 @@
         <v>31</v>
       </c>
       <c r="AG1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" ht="128" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="7">
         <v>2225</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2" s="7">
         <v>3</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="L2" s="8">
         <v>111</v>
       </c>
       <c r="M2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>41</v>
+      <c r="AG2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a second configuration
</commit_message>
<xml_diff>
--- a/gtaa_lab_v1.xlsx
+++ b/gtaa_lab_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamah/Programming/gtaa_nexus7k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07AB19CE-2738-A449-AE92-2CD2B68E11E7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{766155A8-E2CA-354D-9A6A-BE691E54595F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="7700" windowWidth="35920" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,12 +461,951 @@
         </r>
       </text>
     </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{DABC800F-5161-064F-80DB-03C49B6AA865}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vrf context KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">router bgp 65001
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  vrf KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    address-family ipv4 unicast
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">      redistribute direct route-map DIRECT_BGP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{4794447D-D923-EC42-A1FF-3ADFC3D70894}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>description Korean Airlines Back Office</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{03A0EDAE-B5E8-ED4F-9D40-60673A3E0E33}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>rd 65001:1172</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{A0047F72-F31F-DB4D-BBD5-72B173A534D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vrf context KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  address-family ipv4 unicast
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  route-target both 65001:1172</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{CA94A021-796D-D14D-90BB-2777EA645794}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vlan 2177</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{7A21AAD4-9A33-1546-9591-0BB0AB821A93}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>name KE-Cargo-BO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{7656B782-99C0-4847-8CE8-3606D1BA3FA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">de Guzman,Christian:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">interface vlan 2177
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">desc Back Office
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vrf member KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>no ip redirects</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{F676DBCA-30BB-2941-8847-246B282FF8EE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">interface vlan 2177
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ip address 172.16.2.26/29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{CB938522-FA93-594E-81B4-85F0A5DBF4F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">interface vlan 2177
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ip address 172.16.2.27/29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{3ADBF28F-7F3E-354E-A7DF-F89BA35CDDFC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+interface vlan 2177
+hsrp 7
+ip 172.16.2.25
+timers 1 5
+preempt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{6F61033C-C4D3-BC46-9D3D-2BCB5B31D09A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">@111
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">spanning-tree vlan 2177 priority 4096
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">@112
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">spanning-tree vlan 2177 priority 8192
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">interface vlan 2177
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">hsrp 7
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>priority 90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{1D107869-4645-634F-BBBA-6E86FF2003D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vrf context KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  ip route 10.155.108.0/24 Vlan2177 172.16.2.30
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  ip route 10.201.7.0/24 Vlan2177 172.16.2.30
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">router bgp 65001
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  vrf KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    address-family ipv4 unicast
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">      redistribute static route-map STATIC_BGP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{823EA824-8868-4E4A-999C-8F93E9A24E95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">interface vlan 2177
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ip address 172.16.2.26/29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{12F59B04-6D84-D549-ACE7-1D6C21490717}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+interface vlan 2177
+ip address 172.16.2.27/29</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{A4F5D7ED-1606-6E48-B276-9C43DF26DC97}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">interface vlan 2177
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">hsrp 7
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ip 172.16.2.25
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">timers 1 5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>preempt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{02511C07-D2B0-5644-8276-FC199EA0AF89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">@111
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">spanning-tree vlan 2177 priority 4096
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">@112
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">spanning-tree vlan 2177 priority 8192
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">interface vlan 2177
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">hsrp 7
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>priority 90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{61998D17-DE74-BB42-9AF3-2E165AD5A7A3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vrf context KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  ip route 10.155.108.0/24 Vlan2177 172.16.2.30
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  ip route 10.201.7.0/24 Vlan2177 172.16.2.30
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">router bgp 65001
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  vrf KE-CARGO-BO
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    address-family ipv4 unicast
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">      redistribute static route-map STATIC_BGP</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>VRF-Name</t>
   </si>
@@ -596,13 +1535,32 @@
   </si>
   <si>
     <t>Execute</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>KE-CARGO-BO</t>
+  </si>
+  <si>
+    <t>Korean Airlines Back Office</t>
+  </si>
+  <si>
+    <t>KE-Cargo-BO</t>
+  </si>
+  <si>
+    <t>Back Office</t>
+  </si>
+  <si>
+    <t>10.155.108.0/24 Vlan2177 172.16.2.30
+10.201.7.0/24 Vlan2177 172.16.2.30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -620,6 +1578,19 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -668,7 +1639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -692,6 +1663,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1008,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,6 +2147,74 @@
         <v>39</v>
       </c>
     </row>
+    <row r="3" spans="1:34" ht="128" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7">
+        <v>2177</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="7">
+        <v>7</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="8">
+        <v>111</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="9">
+        <v>106</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>